<commit_message>
update uml + template
</commit_message>
<xml_diff>
--- a/Database/ccfa_database.xlsx
+++ b/Database/ccfa_database.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="100">
   <si>
     <t>Table</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mapping Class </t>
+  </si>
+  <si>
+    <t>www.kimlabs.com</t>
   </si>
 </sst>
 </file>
@@ -625,6 +628,282 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -648,282 +927,6 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -938,19 +941,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:L66" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="12" tableBorderDxfId="13">
-  <autoFilter ref="B2:L66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:L68" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
+  <autoFilter ref="B2:L68"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Table" dataDxfId="11"/>
-    <tableColumn id="2" name="Mapping Class " dataDxfId="10"/>
-    <tableColumn id="3" name="Description " dataDxfId="9"/>
-    <tableColumn id="4" name="Column" dataDxfId="8"/>
-    <tableColumn id="5" name="Data Type" dataDxfId="7"/>
-    <tableColumn id="6" name="Length" dataDxfId="6"/>
-    <tableColumn id="7" name="Allow Null" dataDxfId="5"/>
-    <tableColumn id="8" name="Primary Key" dataDxfId="4"/>
-    <tableColumn id="9" name="Foreign Key" dataDxfId="3"/>
-    <tableColumn id="10" name="Unique" dataDxfId="2"/>
+    <tableColumn id="1" name="Table" dataDxfId="9"/>
+    <tableColumn id="2" name="Mapping Class " dataDxfId="8"/>
+    <tableColumn id="3" name="Description " dataDxfId="7"/>
+    <tableColumn id="4" name="Column" dataDxfId="6"/>
+    <tableColumn id="5" name="Data Type" dataDxfId="5"/>
+    <tableColumn id="6" name="Length" dataDxfId="4"/>
+    <tableColumn id="7" name="Allow Null" dataDxfId="3"/>
+    <tableColumn id="8" name="Primary Key" dataDxfId="2"/>
+    <tableColumn id="9" name="Foreign Key" dataDxfId="1"/>
+    <tableColumn id="10" name="Unique" dataDxfId="0"/>
     <tableColumn id="11" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1220,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L66"/>
+  <dimension ref="B2:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="E39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,13 +1495,13 @@
       <c r="C13" s="9"/>
       <c r="D13" s="11"/>
       <c r="E13" s="10" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="11">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>12</v>
@@ -1506,14 +1509,16 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="12"/>
-      <c r="L13" s="23"/>
+      <c r="L13" s="28" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="11"/>
       <c r="E14" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>24</v>
@@ -1534,7 +1539,7 @@
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="10" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>24</v>
@@ -1555,7 +1560,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="11"/>
       <c r="E16" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>24</v>
@@ -1576,13 +1581,13 @@
       <c r="C17" s="9"/>
       <c r="D17" s="11"/>
       <c r="E17" s="10" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G17" s="11">
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>12</v>
@@ -1597,133 +1602,135 @@
       <c r="C18" s="9"/>
       <c r="D18" s="11"/>
       <c r="E18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="11">
+        <v>125</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="23"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="23"/>
-    </row>
-    <row r="19" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="24"/>
-    </row>
-    <row r="20" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="G19" s="11"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="23"/>
+    </row>
+    <row r="20" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="24"/>
+    </row>
+    <row r="21" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C21" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E21" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="23"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="11">
-        <v>25</v>
-      </c>
+      <c r="G21" s="11"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="I21" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="J21" s="9"/>
-      <c r="K21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="K21" s="12"/>
+      <c r="L21" s="23"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
       <c r="D22" s="11"/>
       <c r="E22" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="G22" s="11">
+        <v>25</v>
+      </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K22" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
       <c r="D23" s="11"/>
       <c r="E23" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="11">
-        <v>25</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G23" s="11"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="12"/>
-      <c r="L23" s="23"/>
+      <c r="L23" s="25" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
       <c r="D24" s="11"/>
       <c r="E24" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G24" s="11">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
@@ -1736,46 +1743,48 @@
       <c r="C25" s="9"/>
       <c r="D25" s="11"/>
       <c r="E25" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="G25" s="11">
+        <v>50</v>
+      </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="12"/>
-      <c r="L25" s="23" t="s">
-        <v>75</v>
-      </c>
+      <c r="L25" s="23"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="11"/>
       <c r="E26" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="12"/>
-      <c r="L26" s="23"/>
+      <c r="L26" s="23" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
       <c r="D27" s="11"/>
       <c r="E27" s="10" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="9"/>
@@ -1789,17 +1798,15 @@
       <c r="C28" s="9"/>
       <c r="D28" s="11"/>
       <c r="E28" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="J28" s="9"/>
       <c r="K28" s="12"/>
       <c r="L28" s="23"/>
     </row>
@@ -1808,156 +1815,156 @@
       <c r="C29" s="9"/>
       <c r="D29" s="11"/>
       <c r="E29" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="11"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" s="12"/>
+      <c r="L29" s="23"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F30" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G30" s="11">
         <v>255</v>
       </c>
-      <c r="H29" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="23" t="s">
+      <c r="H30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="24"/>
-    </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="24"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C32" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D32" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F32" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J31" s="9"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="23"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G32" s="11">
-        <v>125</v>
-      </c>
+      <c r="G32" s="11"/>
       <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="I32" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="J32" s="9"/>
       <c r="K32" s="12"/>
-      <c r="L32" s="23" t="s">
-        <v>71</v>
-      </c>
+      <c r="L32" s="23"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
       <c r="C33" s="9"/>
       <c r="D33" s="11"/>
       <c r="E33" s="10" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="G33" s="11">
+        <v>125</v>
+      </c>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
-      <c r="J33" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="J33" s="9"/>
       <c r="K33" s="12"/>
-      <c r="L33" s="23"/>
+      <c r="L33" s="23" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="26"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K34" s="12"/>
+      <c r="L34" s="23"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="26"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C36" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D36" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E36" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="11"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J35" s="9"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="23"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="10" t="s">
-        <v>79</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G36" s="11"/>
       <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="I36" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" s="9"/>
       <c r="K36" s="12"/>
       <c r="L36" s="23"/>
     </row>
@@ -1966,7 +1973,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="11"/>
       <c r="E37" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>11</v>
@@ -1985,75 +1992,73 @@
       <c r="C38" s="9"/>
       <c r="D38" s="11"/>
       <c r="E38" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="G38" s="11"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
+      <c r="J38" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="K38" s="12"/>
-      <c r="L38" s="27">
+      <c r="L38" s="23"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="8"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G39" s="11"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="27">
         <v>43728.456944444442</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="26"/>
-    </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="26"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C41" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D41" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E41" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J40" s="9"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="23"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="8"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G41" s="11">
-        <v>25</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I41" s="9"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="J41" s="9"/>
       <c r="K41" s="12"/>
       <c r="L41" s="23"/>
@@ -2063,56 +2068,58 @@
       <c r="C42" s="9"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G42" s="11">
-        <v>125</v>
-      </c>
-      <c r="H42" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="12"/>
       <c r="L42" s="23"/>
     </row>
-    <row r="43" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="9"/>
       <c r="D43" s="11"/>
       <c r="E43" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G43" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="G43" s="11">
+        <v>125</v>
+      </c>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="12"/>
-      <c r="L43" s="25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L43" s="23"/>
+    </row>
+    <row r="44" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="9"/>
       <c r="D44" s="11"/>
       <c r="E44" s="10" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="12"/>
-      <c r="L44" s="27">
-        <v>43728.456944444442</v>
+      <c r="L44" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
@@ -2120,73 +2127,73 @@
       <c r="C45" s="9"/>
       <c r="D45" s="11"/>
       <c r="E45" s="10" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
-      <c r="J45" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="J45" s="9"/>
       <c r="K45" s="12"/>
-      <c r="L45" s="23"/>
+      <c r="L45" s="27">
+        <v>43728.456944444442</v>
+      </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="13"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="24"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="11"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K46" s="12"/>
+      <c r="L46" s="23"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="13"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="24"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C48" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D48" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E48" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F48" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G47" s="11"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J47" s="9"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="23"/>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="8"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G48" s="11">
-        <v>25</v>
-      </c>
+      <c r="G48" s="11"/>
       <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
+      <c r="I48" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="J48" s="9"/>
       <c r="K48" s="12"/>
       <c r="L48" s="23"/>
@@ -2196,13 +2203,13 @@
       <c r="C49" s="9"/>
       <c r="D49" s="11"/>
       <c r="E49" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G49" s="11">
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
@@ -2215,12 +2222,14 @@
       <c r="C50" s="9"/>
       <c r="D50" s="11"/>
       <c r="E50" s="10" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G50" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="G50" s="11">
+        <v>125</v>
+      </c>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
@@ -2232,74 +2241,72 @@
       <c r="C51" s="9"/>
       <c r="D51" s="11"/>
       <c r="E51" s="10" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="9"/>
       <c r="I51" s="9"/>
-      <c r="J51" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="J51" s="9"/>
       <c r="K51" s="12"/>
       <c r="L51" s="23"/>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="13"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="16"/>
-      <c r="L52" s="24"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="11"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="12"/>
+      <c r="L52" s="23"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="13"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="24"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C54" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D53" s="20" t="s">
+      <c r="D54" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E54" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" s="11"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J53" s="9"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="23"/>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54" s="8"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="10" t="s">
-        <v>79</v>
       </c>
       <c r="F54" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G54" s="11"/>
       <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="I54" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J54" s="9"/>
       <c r="K54" s="12"/>
       <c r="L54" s="23"/>
     </row>
@@ -2308,7 +2315,7 @@
       <c r="C55" s="9"/>
       <c r="D55" s="11"/>
       <c r="E55" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>11</v>
@@ -2323,220 +2330,257 @@
       <c r="L55" s="23"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B56" s="13"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="16"/>
-      <c r="L56" s="24"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="11"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K56" s="12"/>
+      <c r="L56" s="23"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="13"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="24"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C58" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D57" s="20" t="s">
+      <c r="D58" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E58" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F58" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="11"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J57" s="9"/>
-      <c r="K57" s="12"/>
-      <c r="L57" s="23"/>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="8"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F58" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G58" s="11">
-        <v>125</v>
-      </c>
+      <c r="G58" s="11"/>
       <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
+      <c r="I58" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="J58" s="9"/>
       <c r="K58" s="12"/>
-      <c r="L58" s="28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L58" s="23"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="8"/>
       <c r="C59" s="9"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G59" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="G59" s="11">
+        <v>125</v>
+      </c>
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="12"/>
-      <c r="L59" s="25" t="s">
-        <v>77</v>
+      <c r="L59" s="28" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B60" s="13"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="16"/>
-      <c r="L60" s="24"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G60" s="11"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="28"/>
     </row>
     <row r="61" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B61" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>63</v>
-      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="11"/>
       <c r="E61" s="10" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="9"/>
-      <c r="I61" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="12"/>
-      <c r="L61" s="23"/>
+      <c r="L61" s="25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B62" s="8"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G62" s="11">
-        <v>50</v>
-      </c>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="L62" s="23"/>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B63" s="8"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="11"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="16"/>
+      <c r="L62" s="24"/>
+    </row>
+    <row r="63" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B63" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="E63" s="10" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G63" s="11">
-        <v>50</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G63" s="11"/>
       <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
+      <c r="I63" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="J63" s="9"/>
       <c r="K63" s="12"/>
       <c r="L63" s="23"/>
     </row>
-    <row r="64" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
       <c r="C64" s="9"/>
       <c r="D64" s="11"/>
       <c r="E64" s="10" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G64" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="G64" s="11">
+        <v>50</v>
+      </c>
       <c r="H64" s="9"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="K64" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L64" s="23"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" s="8"/>
       <c r="C65" s="9"/>
       <c r="D65" s="11"/>
       <c r="E65" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G65" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="G65" s="11">
+        <v>50</v>
+      </c>
       <c r="H65" s="9"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="12"/>
-      <c r="L65" s="25" t="s">
+      <c r="L65" s="23"/>
+    </row>
+    <row r="66" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B66" s="8"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" s="11"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B67" s="8"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" s="11"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B66" s="29"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="30"/>
-      <c r="G66" s="31"/>
-      <c r="H66" s="30"/>
-      <c r="I66" s="30"/>
-      <c r="J66" s="30"/>
-      <c r="K66" s="33"/>
-      <c r="L66" s="34"/>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B68" s="29"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="31"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="30"/>
+      <c r="J68" s="30"/>
+      <c r="K68" s="33"/>
+      <c r="L68" s="34"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L58" r:id="rId1"/>
+    <hyperlink ref="L59" r:id="rId1"/>
+    <hyperlink ref="L13" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>